<commit_message>
Fix sim, number match, space line break, and master data
sim = 80
</commit_message>
<xml_diff>
--- a/xls/14001-108-240018314(2)_1.xlsx
+++ b/xls/14001-108-240018314(2)_1.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ค่ารักษาพยาบาลจากอุบัติเหตุทั่วไป (ไม่รวม มอเตอร์ไซด์)</t>
+          <t>ค่ารักษาพยาบาลจากอุบัติเหตุทั่วไป (ไม่รวมมอเตอร์ไซด์)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -523,17 +523,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ค่ารักษาพยาบาลจากอุบัติเหตุทั่วไป (ไม่รวม มอเตอร์ไซด์)</t>
+          <t>ค่ารักษาพยาบาลจากอุบัติเหตุทั่วไป (ไม่รวมมอเตอร์ไซด์)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>100</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ชดเชยค่ารักษาพยาบาลเนื่องจากอุบัติเหตุ</t>
+          <t>ค่ารักษาพยาบาลจากอุบัติเหตุมอเตอร์ไซด์</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>100</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>